<commit_message>
fixed list benifis f and arab 17-06-2024
</commit_message>
<xml_diff>
--- a/ListBenefisiersFr.xlsx
+++ b/ListBenefisiersFr.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Houda\Documents\SDL3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DFC5A0-6A19-49CB-A6FE-24CE76D2AC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3516DA82-8EFA-45C9-9516-FB9719D3919A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="913" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="913" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="اقل احتياطية" sheetId="50" r:id="rId1"/>
-    <sheet name="أكبر احتياطية" sheetId="49" r:id="rId2"/>
-    <sheet name="اقل" sheetId="48" r:id="rId3"/>
-    <sheet name="أكبر" sheetId="47" r:id="rId4"/>
+    <sheet name="Moin" sheetId="48" r:id="rId1"/>
+    <sheet name="Plus" sheetId="47" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">اقل!$A$6:$AD$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'اقل احتياطية'!$A$6:$AD$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">أكبر!$A$6:$AC$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'أكبر احتياطية'!$A$6:$AC$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">اقل!$A$1:$AD$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'اقل احتياطية'!$A$1:$AD$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">أكبر!$A$1:$AD$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'أكبر احتياطية'!$A$1:$AD$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moin!$A$6:$AD$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plus!$A$6:$AC$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Moin!$A$1:$AD$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Plus!$A$1:$AD$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>République Algérienne Démocratique et Populaire</t>
   </si>
@@ -140,18 +134,12 @@
   <si>
     <t>La liste nominale définitive des bénéficiaires de logements locatifs publics (quota 2021/87) pour la commune de Taybat (groupe de plus de 35 ans), quantité : 35</t>
   </si>
-  <si>
-    <t xml:space="preserve">Liste nominale de réserve des bénéficiaires de logements sociaux locatifs (quota 2021/87) pour la commune de Taybat (groupe de plus de 35 ans), nombre : 10 </t>
-  </si>
-  <si>
-    <t>Liste nominale de réserve des bénéficiaires des logements sociaux locatifs (quota 2021/87) pour la commune de Taybat (catégorie moins de 35 ans), numéro : 10</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,13 +323,6 @@
       <charset val="178"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color theme="1" tint="0.249977111117893"/>
@@ -369,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -389,15 +370,6 @@
       </top>
       <bottom style="double">
         <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -471,7 +443,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -482,223 +454,134 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="21" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="22" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="22" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="25" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="27" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="26" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -712,7 +595,7 @@
     <cellStyle name="Style 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Style 6" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="171">
+  <dxfs count="101">
     <dxf>
       <font>
         <b/>
@@ -4230,2398 +4113,6 @@
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Mohammad Head"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Mohammad Head"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Mohammad Head"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF008600"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFE101C6"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF008600"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF660066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1" tint="0.249977111117893"/>
-        <name val="Mohammad Bold Normal"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Mohammad Head"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Mohammad Head"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF4343FF"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFE101C6"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF0000B4"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF008600"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Mohammad Head"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF008600"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFE101C6"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF008600"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF660066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF2525FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top style="double">
-          <color indexed="64"/>
-        </top>
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1" tint="0.249977111117893"/>
-        <name val="Mohammad Bold Normal"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="double">
-          <color indexed="64"/>
-        </left>
-        <right style="double">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6637,84 +4128,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="MoisTableA" displayName="MoisTableA" ref="A6:AD7" totalsRowShown="0" headerRowDxfId="170" dataDxfId="168" headerRowBorderDxfId="169" tableBorderDxfId="167" totalsRowBorderDxfId="166">
-  <autoFilter ref="A6:AD7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Classement" dataDxfId="165"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Numéro de dossier" dataDxfId="164"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Date de dépôt" dataDxfId="163"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Nom" dataDxfId="162"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Prenom" dataDxfId="161"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Sexe" dataDxfId="160"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date de naissance" dataDxfId="159"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Numéro d'acte de naissance" dataDxfId="158"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commune de naissance" dataDxfId="157"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Situation familiale" dataDxfId="156"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Prenom du père" dataDxfId="155"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Nom de la Mere" dataDxfId="154"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Prenom de la Mere" dataDxfId="153"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Adresse" dataDxfId="152"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Prénom du conjoint" dataDxfId="151"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Nom du conjoint" dataDxfId="150"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Date de naissance du conjoint" dataDxfId="149"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Numéro d'acte de naissance conjoint" dataDxfId="148"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Commune de naissance Conjoint" dataDxfId="147"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Prenom du père Conjoint" dataDxfId="146"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Nom de la Mere Conjoint" dataDxfId="145"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Prenom de la Mere Conjoint" dataDxfId="144"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="groupe de (plus ou moins) de 35 ans" dataDxfId="143"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Le niveau de revenu" dataDxfId="142"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Conditions de logement" dataDxfId="141"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Note Situation familiale" dataDxfId="140"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Ancienneté de la demande de logement" dataDxfId="139"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="le total_x000a_" dataDxfId="138"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Remarque" dataDxfId="137"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Photo" dataDxfId="136"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="PlusTableA" displayName="PlusTableA" ref="A6:AD7" totalsRowShown="0" headerRowDxfId="135" dataDxfId="133" headerRowBorderDxfId="134" tableBorderDxfId="132" totalsRowBorderDxfId="131">
-  <autoFilter ref="A6:AD7" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Classement" dataDxfId="130"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Numéro de dossier" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Date de dépôt" dataDxfId="128"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Nom" dataDxfId="127"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Prenom" dataDxfId="126"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Sexe" dataDxfId="125"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Date de naissance" dataDxfId="124"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Numéro d'acte de naissance" dataDxfId="123"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Commune de naissance" dataDxfId="122"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Situation familiale" dataDxfId="121"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Prenom du père" dataDxfId="120"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Nom de la Mere" dataDxfId="119"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Prenom de la Mere" dataDxfId="118"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Adresse" dataDxfId="117"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Prénom du conjoint" dataDxfId="116"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Nom du conjoint" dataDxfId="115"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Date de naissance du conjoint" dataDxfId="114"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Numéro d'acte de naissance conjoint" dataDxfId="113"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Commune de naissance Conjoint" dataDxfId="112"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Prenom du père Conjoint" dataDxfId="111"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Nom de la Mere Conjoint" dataDxfId="110"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Prenom de la Mere Conjoint" dataDxfId="109"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="groupe de (plus ou moins) de 35 ans" dataDxfId="108"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Le niveau de revenu" dataDxfId="107"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Conditions de logement" dataDxfId="106"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="Note Situation familiale" dataDxfId="105"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Ancienneté de la demande de logement" dataDxfId="104"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="le total_x000a_" dataDxfId="103"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Remarque" dataDxfId="102"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Photo" dataDxfId="101"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="MoinTable" displayName="MoinTable" ref="A6:AD7" totalsRowShown="0" headerRowDxfId="98" headerRowBorderDxfId="97" tableBorderDxfId="96" totalsRowBorderDxfId="95">
   <autoFilter ref="A6:AD7" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="30">
@@ -6753,7 +4166,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="PlusTable" displayName="PlusTable" ref="A6:AD7" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <autoFilter ref="A6:AD7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AD7">
@@ -7081,685 +4494,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AD7"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" customWidth="1"/>
-    <col min="14" max="14" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="25" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" customWidth="1"/>
-    <col min="18" max="18" width="36.42578125" customWidth="1"/>
-    <col min="19" max="19" width="46.140625" customWidth="1"/>
-    <col min="20" max="20" width="34" customWidth="1"/>
-    <col min="21" max="21" width="30.42578125" customWidth="1"/>
-    <col min="22" max="22" width="28.28515625" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" customWidth="1"/>
-    <col min="28" max="28" width="16.7109375" customWidth="1"/>
-    <col min="29" max="30" width="30.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
-    </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A2" s="48"/>
-      <c r="B2" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-    </row>
-    <row r="3" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A3" s="48"/>
-      <c r="B3" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="48"/>
-      <c r="AC3" s="48"/>
-      <c r="AD3" s="48"/>
-    </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A4" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-    </row>
-    <row r="5" spans="1:30" ht="49.5" customHeight="1">
-      <c r="A5" s="51"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="51"/>
-      <c r="Z5" s="51"/>
-      <c r="AA5" s="51"/>
-      <c r="AB5" s="51"/>
-      <c r="AC5" s="51"/>
-      <c r="AD5" s="51"/>
-    </row>
-    <row r="6" spans="1:30" ht="109.5" customHeight="1" thickBot="1">
-      <c r="A6" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="T6" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="U6" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="V6" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="X6" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y6" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z6" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA6" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB6" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC6" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" s="5" customFormat="1" ht="82.5" customHeight="1" thickTop="1">
-      <c r="A7" s="52">
-        <v>1</v>
-      </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="62"/>
-      <c r="W7" s="65"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="67"/>
-      <c r="Z7" s="68"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="70"/>
-      <c r="AC7" s="71"/>
-      <c r="AD7" s="72"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A4:AD4"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.19685039370078741" bottom="0" header="0.19685039370078741" footer="0"/>
-  <pageSetup paperSize="9" scale="19" orientation="landscape" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:AD7"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="26" zoomScaleNormal="26" zoomScaleSheetLayoutView="26" zoomScalePageLayoutView="32" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
-    <col min="14" max="14" width="92.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" customWidth="1"/>
-    <col min="16" max="16" width="24" customWidth="1"/>
-    <col min="17" max="17" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.5703125" customWidth="1"/>
-    <col min="19" max="19" width="41.140625" customWidth="1"/>
-    <col min="20" max="20" width="32.42578125" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" customWidth="1"/>
-    <col min="22" max="22" width="27.42578125" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" customWidth="1"/>
-    <col min="24" max="24" width="17.140625" customWidth="1"/>
-    <col min="25" max="25" width="17.85546875" customWidth="1"/>
-    <col min="26" max="26" width="17.5703125" customWidth="1"/>
-    <col min="27" max="27" width="19.28515625" customWidth="1"/>
-    <col min="28" max="28" width="22.7109375" customWidth="1"/>
-    <col min="29" max="30" width="29.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
-    </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="B2" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-    </row>
-    <row r="3" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="B3" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-    </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A4" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="75"/>
-      <c r="P4" s="75"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="75"/>
-      <c r="S4" s="75"/>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="75"/>
-      <c r="W4" s="75"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="75"/>
-      <c r="AA4" s="75"/>
-      <c r="AB4" s="75"/>
-      <c r="AC4" s="75"/>
-      <c r="AD4" s="75"/>
-    </row>
-    <row r="5" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="76"/>
-      <c r="U5" s="76"/>
-      <c r="V5" s="76"/>
-      <c r="W5" s="76"/>
-    </row>
-    <row r="6" spans="1:30" s="4" customFormat="1" ht="105.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="T6" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="U6" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="V6" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="X6" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y6" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z6" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA6" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB6" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC6" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" s="5" customFormat="1" ht="83.25" customHeight="1" thickTop="1">
-      <c r="A7" s="27">
-        <v>1</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="39"/>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="40"/>
-      <c r="Z7" s="40"/>
-      <c r="AA7" s="40"/>
-      <c r="AB7" s="40"/>
-      <c r="AC7" s="41"/>
-      <c r="AD7" s="42"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A4:AD4"/>
-    <mergeCell ref="C5:W5"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.19685039370078741" bottom="0" header="0.19685039370078741" footer="0"/>
-  <pageSetup paperSize="9" scale="17" orientation="landscape" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -7793,42 +4533,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="82.5" customHeight="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
     </row>
     <row r="2" spans="1:30" ht="45">
       <c r="A2" s="1"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
@@ -7862,7 +4602,7 @@
     </row>
     <row r="3" spans="1:30" ht="45">
       <c r="A3" s="1"/>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
@@ -7895,164 +4635,164 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="1:30" ht="45">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="73"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
     </row>
     <row r="6" spans="1:30" ht="263.25" thickBot="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="47" t="s">
+      <c r="K6" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="47" t="s">
+      <c r="L6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="47" t="s">
+      <c r="M6" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="47" t="s">
+      <c r="O6" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="47" t="s">
+      <c r="P6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="47" t="s">
+      <c r="Q6" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="47" t="s">
+      <c r="R6" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="47" t="s">
+      <c r="S6" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="47" t="s">
+      <c r="T6" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="U6" s="47" t="s">
+      <c r="U6" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="V6" s="47" t="s">
+      <c r="V6" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="W6" s="47" t="s">
+      <c r="W6" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="X6" s="47" t="s">
+      <c r="X6" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="Y6" s="47" t="s">
+      <c r="Y6" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="Z6" s="47" t="s">
+      <c r="Z6" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="AA6" s="47" t="s">
+      <c r="AA6" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AB6" s="47" t="s">
+      <c r="AB6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AC6" s="47" t="s">
+      <c r="AC6" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AD6" s="47" t="s">
+      <c r="AD6" s="46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="24" thickTop="1">
-      <c r="A7" s="6">
+    <row r="7" spans="1:30" ht="200.1" customHeight="1" thickTop="1">
+      <c r="A7" s="5">
         <v>1</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="25"/>
-      <c r="AD7" s="26"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="24"/>
+      <c r="AD7" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AE126">
@@ -8072,13 +4812,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="L1" zoomScale="26" zoomScaleNormal="26" zoomScaleSheetLayoutView="26" zoomScalePageLayoutView="32" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView view="pageBreakPreview" topLeftCell="H1" zoomScale="26" zoomScaleNormal="26" zoomScaleSheetLayoutView="26" zoomScalePageLayoutView="32" workbookViewId="0">
+      <selection activeCell="H7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -8116,41 +4856,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
     </row>
     <row r="2" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
@@ -8176,7 +4916,7 @@
       <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
@@ -8202,243 +4942,243 @@
       <c r="W3" s="3"/>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="73"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
     </row>
     <row r="5" spans="1:30" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
     </row>
     <row r="6" spans="1:30" s="4" customFormat="1" ht="198" customHeight="1" thickBot="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="47" t="s">
+      <c r="K6" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="47" t="s">
+      <c r="L6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="47" t="s">
+      <c r="M6" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="N6" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="47" t="s">
+      <c r="O6" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="47" t="s">
+      <c r="P6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="47" t="s">
+      <c r="Q6" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="47" t="s">
+      <c r="R6" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="47" t="s">
+      <c r="S6" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="47" t="s">
+      <c r="T6" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="U6" s="47" t="s">
+      <c r="U6" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="V6" s="47" t="s">
+      <c r="V6" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="W6" s="47" t="s">
+      <c r="W6" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="X6" s="47" t="s">
+      <c r="X6" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="Y6" s="47" t="s">
+      <c r="Y6" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="Z6" s="47" t="s">
+      <c r="Z6" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="AA6" s="47" t="s">
+      <c r="AA6" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AB6" s="47" t="s">
+      <c r="AB6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AC6" s="47" t="s">
+      <c r="AC6" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AD6" s="47" t="s">
+      <c r="AD6" s="46" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="200.1" customHeight="1" thickTop="1">
-      <c r="A7" s="27">
+      <c r="A7" s="26">
         <v>1</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="27">
         <v>1</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>1</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>1</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="30">
         <v>1</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="31">
         <v>1</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="32">
         <v>1</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="33">
         <v>1</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="34">
         <v>1</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="31">
         <v>1</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="30">
         <v>1</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="29">
         <v>1</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="30">
         <v>1</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="27">
         <v>1</v>
       </c>
-      <c r="O7" s="36">
+      <c r="O7" s="35">
         <v>1</v>
       </c>
-      <c r="P7" s="37">
+      <c r="P7" s="36">
         <v>1</v>
       </c>
-      <c r="Q7" s="38">
+      <c r="Q7" s="37">
         <v>1</v>
       </c>
-      <c r="R7" s="34">
+      <c r="R7" s="33">
         <v>1</v>
       </c>
-      <c r="S7" s="35">
+      <c r="S7" s="34">
         <v>1</v>
       </c>
-      <c r="T7" s="36">
+      <c r="T7" s="35">
         <v>1</v>
       </c>
-      <c r="U7" s="37">
+      <c r="U7" s="36">
         <v>1</v>
       </c>
-      <c r="V7" s="36">
+      <c r="V7" s="35">
         <v>1</v>
       </c>
-      <c r="W7" s="39">
+      <c r="W7" s="38">
         <v>1</v>
       </c>
-      <c r="X7" s="40">
+      <c r="X7" s="39">
         <v>1</v>
       </c>
-      <c r="Y7" s="40">
+      <c r="Y7" s="39">
         <v>1</v>
       </c>
-      <c r="Z7" s="40">
+      <c r="Z7" s="39">
         <v>1</v>
       </c>
-      <c r="AA7" s="40">
+      <c r="AA7" s="39">
         <v>1</v>
       </c>
-      <c r="AB7" s="40">
+      <c r="AB7" s="39">
         <v>1</v>
       </c>
-      <c r="AC7" s="41">
+      <c r="AC7" s="40">
         <v>1</v>
       </c>
-      <c r="AD7" s="42">
+      <c r="AD7" s="41">
         <v>1</v>
       </c>
     </row>

</xml_diff>